<commit_message>
match add return a list of recommended option
</commit_message>
<xml_diff>
--- a/classification_matching/Matched_Armadale.xlsx
+++ b/classification_matching/Matched_Armadale.xlsx
@@ -1441,7 +1441,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H12" t="inlineStr"/>
@@ -2190,7 +2190,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H21" t="inlineStr"/>
@@ -2605,7 +2605,11 @@
           <t>food, point_of_interest, establishment</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr"/>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Food Production and Preparation</t>
+        </is>
+      </c>
       <c r="H26" t="inlineStr"/>
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr"/>
@@ -2822,7 +2826,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H29" t="inlineStr"/>
@@ -2895,7 +2899,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H30" t="inlineStr"/>
@@ -2968,7 +2972,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H31" t="inlineStr"/>
@@ -3041,7 +3045,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H32" t="inlineStr"/>
@@ -3114,7 +3118,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H33" t="inlineStr"/>
@@ -3268,7 +3272,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H35" t="inlineStr"/>
@@ -3341,7 +3345,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H36" t="inlineStr"/>
@@ -3414,7 +3418,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H37" t="inlineStr"/>
@@ -3560,7 +3564,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H39" t="inlineStr"/>
@@ -3722,7 +3726,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H41" t="inlineStr"/>
@@ -3795,7 +3799,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H42" t="inlineStr"/>
@@ -3868,7 +3872,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H43" t="inlineStr"/>
@@ -4010,7 +4014,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H45" t="inlineStr"/>
@@ -4160,7 +4164,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H47" t="inlineStr"/>
@@ -4233,7 +4237,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H48" t="inlineStr"/>
@@ -4395,7 +4399,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H50" t="inlineStr"/>
@@ -4549,7 +4553,7 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H52" t="inlineStr"/>
@@ -4622,7 +4626,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H53" t="inlineStr"/>
@@ -4849,7 +4853,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H56" t="inlineStr"/>
@@ -4995,7 +4999,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H58" t="inlineStr"/>
@@ -5068,7 +5072,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H59" t="inlineStr"/>
@@ -5141,7 +5145,7 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H60" t="inlineStr"/>
@@ -5214,7 +5218,7 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H61" t="inlineStr"/>
@@ -5287,7 +5291,7 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H62" t="inlineStr"/>
@@ -5360,7 +5364,7 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H63" t="inlineStr"/>
@@ -5433,7 +5437,7 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H64" t="inlineStr"/>
@@ -5506,7 +5510,7 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H65" t="inlineStr"/>
@@ -5579,7 +5583,7 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H66" t="inlineStr"/>
@@ -5652,7 +5656,7 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H67" t="inlineStr"/>
@@ -5802,7 +5806,7 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H69" t="inlineStr"/>
@@ -5875,7 +5879,7 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H70" t="inlineStr"/>
@@ -5948,7 +5952,7 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H71" t="inlineStr"/>
@@ -6175,7 +6179,7 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H74" t="inlineStr"/>
@@ -6248,7 +6252,7 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H75" t="inlineStr"/>
@@ -6398,7 +6402,7 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H77" t="inlineStr"/>
@@ -6548,7 +6552,7 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H79" t="inlineStr"/>
@@ -6621,7 +6625,7 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H80" t="inlineStr"/>
@@ -6694,7 +6698,7 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H81" t="inlineStr"/>
@@ -6767,7 +6771,7 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H82" t="inlineStr"/>
@@ -6840,7 +6844,7 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H83" t="inlineStr"/>
@@ -6913,7 +6917,7 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H84" t="inlineStr"/>
@@ -6982,7 +6986,7 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H85" t="inlineStr"/>
@@ -7051,7 +7055,7 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H86" t="inlineStr"/>
@@ -7118,7 +7122,11 @@
           <t>lawyer, point_of_interest, establishment</t>
         </is>
       </c>
-      <c r="G87" t="inlineStr"/>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
+        </is>
+      </c>
       <c r="H87" t="inlineStr"/>
       <c r="I87" t="inlineStr"/>
       <c r="J87" t="inlineStr"/>
@@ -7185,7 +7193,7 @@
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H88" t="inlineStr"/>
@@ -7254,7 +7262,7 @@
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H89" t="inlineStr"/>
@@ -7323,7 +7331,7 @@
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H90" t="inlineStr"/>
@@ -7392,7 +7400,7 @@
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H91" t="inlineStr"/>
@@ -7461,7 +7469,7 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H92" t="inlineStr"/>
@@ -7530,7 +7538,7 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H93" t="inlineStr"/>
@@ -7672,7 +7680,7 @@
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H95" t="inlineStr"/>
@@ -7741,7 +7749,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H96" t="inlineStr"/>
@@ -7810,7 +7818,7 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H97" t="inlineStr"/>
@@ -7952,7 +7960,7 @@
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H99" t="inlineStr"/>
@@ -8021,7 +8029,7 @@
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H100" t="inlineStr"/>
@@ -8090,7 +8098,7 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H101" t="inlineStr"/>
@@ -8159,7 +8167,7 @@
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H102" t="inlineStr"/>
@@ -8228,7 +8236,7 @@
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H103" t="inlineStr"/>
@@ -8297,7 +8305,7 @@
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H104" t="inlineStr"/>
@@ -8366,7 +8374,7 @@
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H105" t="inlineStr"/>
@@ -8520,7 +8528,7 @@
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H107" t="inlineStr"/>
@@ -8589,7 +8597,7 @@
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H108" t="inlineStr"/>
@@ -8658,7 +8666,7 @@
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H109" t="inlineStr"/>
@@ -8727,7 +8735,7 @@
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H110" t="inlineStr"/>
@@ -8796,7 +8804,7 @@
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H111" t="inlineStr"/>
@@ -8865,7 +8873,7 @@
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H112" t="inlineStr"/>
@@ -8934,7 +8942,7 @@
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H113" t="inlineStr"/>
@@ -9003,7 +9011,7 @@
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H114" t="inlineStr"/>
@@ -9072,7 +9080,7 @@
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H115" t="inlineStr"/>
@@ -9141,7 +9149,7 @@
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H116" t="inlineStr"/>
@@ -9210,7 +9218,7 @@
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H117" t="inlineStr"/>
@@ -9279,7 +9287,7 @@
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H118" t="inlineStr"/>
@@ -9348,7 +9356,7 @@
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H119" t="inlineStr"/>
@@ -9417,7 +9425,7 @@
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H120" t="inlineStr"/>
@@ -9486,7 +9494,7 @@
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H121" t="inlineStr"/>
@@ -9555,7 +9563,7 @@
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H122" t="inlineStr"/>
@@ -9624,7 +9632,7 @@
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H123" t="inlineStr"/>
@@ -9693,7 +9701,7 @@
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H124" t="inlineStr"/>
@@ -9762,7 +9770,7 @@
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H125" t="inlineStr"/>
@@ -9831,7 +9839,7 @@
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H126" t="inlineStr"/>
@@ -9900,7 +9908,7 @@
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H127" t="inlineStr"/>
@@ -9969,7 +9977,7 @@
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H128" t="inlineStr"/>
@@ -10038,7 +10046,7 @@
       </c>
       <c r="G129" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H129" t="inlineStr"/>
@@ -10107,7 +10115,7 @@
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H130" t="inlineStr"/>
@@ -10249,7 +10257,7 @@
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H132" t="inlineStr"/>
@@ -10322,7 +10330,7 @@
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H133" t="inlineStr"/>
@@ -10630,7 +10638,7 @@
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H137" t="inlineStr"/>
@@ -10703,7 +10711,7 @@
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H138" t="inlineStr"/>
@@ -10776,7 +10784,7 @@
       </c>
       <c r="G139" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H139" t="inlineStr"/>
@@ -10922,7 +10930,7 @@
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H141" t="inlineStr"/>
@@ -11157,7 +11165,7 @@
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H144" t="inlineStr"/>
@@ -11447,7 +11455,11 @@
           <t>food, point_of_interest, store, establishment</t>
         </is>
       </c>
-      <c r="G148" t="inlineStr"/>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>Food Production and Preparation</t>
+        </is>
+      </c>
       <c r="H148" t="inlineStr"/>
       <c r="I148" t="inlineStr"/>
       <c r="J148" t="inlineStr"/>
@@ -11599,7 +11611,7 @@
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H150" t="inlineStr"/>
@@ -11887,7 +11899,7 @@
       </c>
       <c r="G154" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H154" t="inlineStr"/>
@@ -11960,7 +11972,7 @@
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H155" t="inlineStr"/>
@@ -12187,7 +12199,7 @@
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H158" t="inlineStr"/>
@@ -12258,7 +12270,11 @@
           <t>car_repair, store, point_of_interest, establishment</t>
         </is>
       </c>
-      <c r="G159" t="inlineStr"/>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>FOOD RETAIL</t>
+        </is>
+      </c>
       <c r="H159" t="inlineStr"/>
       <c r="I159" t="inlineStr"/>
       <c r="J159" t="inlineStr"/>
@@ -12402,7 +12418,7 @@
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H161" t="inlineStr"/>
@@ -12629,7 +12645,7 @@
       </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H164" t="inlineStr"/>
@@ -12700,7 +12716,11 @@
           <t>food, point_of_interest, establishment</t>
         </is>
       </c>
-      <c r="G165" t="inlineStr"/>
+      <c r="G165" t="inlineStr">
+        <is>
+          <t>Food Production and Preparation</t>
+        </is>
+      </c>
       <c r="H165" t="inlineStr"/>
       <c r="I165" t="inlineStr"/>
       <c r="J165" t="inlineStr"/>
@@ -12840,7 +12860,7 @@
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H167" t="inlineStr"/>
@@ -12911,7 +12931,11 @@
           <t>food, point_of_interest, establishment</t>
         </is>
       </c>
-      <c r="G168" t="inlineStr"/>
+      <c r="G168" t="inlineStr">
+        <is>
+          <t>Food Production and Preparation</t>
+        </is>
+      </c>
       <c r="H168" t="inlineStr"/>
       <c r="I168" t="inlineStr"/>
       <c r="J168" t="inlineStr"/>
@@ -12982,7 +13006,7 @@
       </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H169" t="inlineStr"/>
@@ -13055,7 +13079,7 @@
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H170" t="inlineStr"/>
@@ -13128,7 +13152,7 @@
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H171" t="inlineStr"/>
@@ -13290,7 +13314,7 @@
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H173" t="inlineStr"/>
@@ -13363,7 +13387,7 @@
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H174" t="inlineStr"/>
@@ -13578,7 +13602,7 @@
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H177" t="inlineStr"/>
@@ -13645,7 +13669,11 @@
           <t>food, point_of_interest, establishment</t>
         </is>
       </c>
-      <c r="G178" t="inlineStr"/>
+      <c r="G178" t="inlineStr">
+        <is>
+          <t>Food Production and Preparation</t>
+        </is>
+      </c>
       <c r="H178" t="inlineStr"/>
       <c r="I178" t="inlineStr"/>
       <c r="J178" t="inlineStr"/>
@@ -14022,7 +14050,11 @@
           <t>food, point_of_interest, establishment</t>
         </is>
       </c>
-      <c r="G183" t="inlineStr"/>
+      <c r="G183" t="inlineStr">
+        <is>
+          <t>Food Production and Preparation</t>
+        </is>
+      </c>
       <c r="H183" t="inlineStr"/>
       <c r="I183" t="inlineStr"/>
       <c r="J183" t="inlineStr"/>
@@ -14782,7 +14814,7 @@
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H193" t="inlineStr"/>
@@ -15001,7 +15033,7 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H196" t="inlineStr"/>
@@ -15366,7 +15398,7 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H201" t="inlineStr"/>
@@ -15512,7 +15544,7 @@
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H203" t="inlineStr"/>
@@ -15585,7 +15617,7 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H204" t="inlineStr"/>
@@ -16207,7 +16239,11 @@
           <t>grocery_or_supermarket, food, store, point_of_interest, establishment</t>
         </is>
       </c>
-      <c r="G212" t="inlineStr"/>
+      <c r="G212" t="inlineStr">
+        <is>
+          <t>Food Production and Preparation</t>
+        </is>
+      </c>
       <c r="H212" t="inlineStr"/>
       <c r="I212" t="inlineStr"/>
       <c r="J212" t="inlineStr"/>
@@ -16888,7 +16924,11 @@
           <t>grocery_or_supermarket, store, food, point_of_interest, establishment</t>
         </is>
       </c>
-      <c r="G221" t="inlineStr"/>
+      <c r="G221" t="inlineStr">
+        <is>
+          <t>FOOD RETAIL</t>
+        </is>
+      </c>
       <c r="H221" t="inlineStr"/>
       <c r="I221" t="inlineStr"/>
       <c r="J221" t="inlineStr"/>
@@ -17105,7 +17145,7 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H224" t="inlineStr"/>
@@ -17405,7 +17445,7 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H228" t="inlineStr"/>
@@ -17474,7 +17514,7 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H229" t="inlineStr"/>
@@ -17693,7 +17733,7 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H232" t="inlineStr"/>
@@ -18905,7 +18945,7 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H248" t="inlineStr"/>
@@ -19049,7 +19089,11 @@
           <t>food, point_of_interest, establishment</t>
         </is>
       </c>
-      <c r="G250" t="inlineStr"/>
+      <c r="G250" t="inlineStr">
+        <is>
+          <t>Food Production and Preparation</t>
+        </is>
+      </c>
       <c r="H250" t="inlineStr"/>
       <c r="I250" t="inlineStr"/>
       <c r="J250" t="inlineStr"/>
@@ -19270,7 +19314,7 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H253" t="inlineStr"/>
@@ -19491,7 +19535,11 @@
           <t>food, point_of_interest, establishment</t>
         </is>
       </c>
-      <c r="G256" t="inlineStr"/>
+      <c r="G256" t="inlineStr">
+        <is>
+          <t>Food Production and Preparation</t>
+        </is>
+      </c>
       <c r="H256" t="inlineStr"/>
       <c r="I256" t="inlineStr"/>
       <c r="J256" t="inlineStr"/>
@@ -27363,7 +27411,11 @@
           <t>grocery_or_supermarket, food, store, point_of_interest, establishment</t>
         </is>
       </c>
-      <c r="G356" t="inlineStr"/>
+      <c r="G356" t="inlineStr">
+        <is>
+          <t>Food Production and Preparation</t>
+        </is>
+      </c>
       <c r="H356" t="inlineStr"/>
       <c r="I356" t="inlineStr"/>
       <c r="J356" t="inlineStr"/>
@@ -27912,7 +27964,7 @@
       </c>
       <c r="G363" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H363" t="inlineStr"/>
@@ -28228,7 +28280,7 @@
       </c>
       <c r="G367" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H367" t="inlineStr"/>
@@ -28617,7 +28669,7 @@
       </c>
       <c r="G372" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H372" t="inlineStr"/>
@@ -29421,7 +29473,11 @@
           <t>grocery_or_supermarket, food, point_of_interest, store, establishment</t>
         </is>
       </c>
-      <c r="G382" t="inlineStr"/>
+      <c r="G382" t="inlineStr">
+        <is>
+          <t>Food Production and Preparation</t>
+        </is>
+      </c>
       <c r="H382" t="inlineStr"/>
       <c r="I382" t="inlineStr"/>
       <c r="J382" t="inlineStr"/>
@@ -29652,7 +29708,11 @@
           <t>food, store, point_of_interest, establishment</t>
         </is>
       </c>
-      <c r="G385" t="inlineStr"/>
+      <c r="G385" t="inlineStr">
+        <is>
+          <t>Food Production and Preparation</t>
+        </is>
+      </c>
       <c r="H385" t="inlineStr"/>
       <c r="I385" t="inlineStr"/>
       <c r="J385" t="inlineStr"/>
@@ -29972,7 +30032,11 @@
           <t>grocery_or_supermarket, point_of_interest, store, food, establishment</t>
         </is>
       </c>
-      <c r="G389" t="inlineStr"/>
+      <c r="G389" t="inlineStr">
+        <is>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
+        </is>
+      </c>
       <c r="H389" t="inlineStr"/>
       <c r="I389" t="inlineStr"/>
       <c r="J389" t="inlineStr"/>
@@ -30041,12 +30105,28 @@
           <t>grocery_or_supermarket, supermarket, store, point_of_interest, food, establishment</t>
         </is>
       </c>
-      <c r="G390" t="inlineStr"/>
-      <c r="H390" t="inlineStr"/>
+      <c r="G390" t="inlineStr">
+        <is>
+          <t>FOOD RETAIL</t>
+        </is>
+      </c>
+      <c r="H390" t="inlineStr">
+        <is>
+          <t>Supermarket/grocery store</t>
+        </is>
+      </c>
       <c r="I390" t="inlineStr"/>
-      <c r="J390" t="inlineStr"/>
+      <c r="J390" t="inlineStr">
+        <is>
+          <t>Supermarket</t>
+        </is>
+      </c>
       <c r="K390" t="inlineStr"/>
-      <c r="L390" t="inlineStr"/>
+      <c r="L390" t="inlineStr">
+        <is>
+          <t>A1.01</t>
+        </is>
+      </c>
       <c r="M390" t="inlineStr"/>
       <c r="N390" t="n">
         <v>-32.1194384</v>
@@ -30187,7 +30267,11 @@
           <t>food, point_of_interest, store, establishment</t>
         </is>
       </c>
-      <c r="G392" t="inlineStr"/>
+      <c r="G392" t="inlineStr">
+        <is>
+          <t>Food Production and Preparation</t>
+        </is>
+      </c>
       <c r="H392" t="inlineStr"/>
       <c r="I392" t="inlineStr"/>
       <c r="J392" t="inlineStr"/>
@@ -30256,12 +30340,28 @@
           <t>grocery_or_supermarket, supermarket, food, point_of_interest, store, establishment</t>
         </is>
       </c>
-      <c r="G393" t="inlineStr"/>
-      <c r="H393" t="inlineStr"/>
+      <c r="G393" t="inlineStr">
+        <is>
+          <t>FOOD RETAIL</t>
+        </is>
+      </c>
+      <c r="H393" t="inlineStr">
+        <is>
+          <t>Supermarket/grocery store</t>
+        </is>
+      </c>
       <c r="I393" t="inlineStr"/>
-      <c r="J393" t="inlineStr"/>
+      <c r="J393" t="inlineStr">
+        <is>
+          <t>Supermarket</t>
+        </is>
+      </c>
       <c r="K393" t="inlineStr"/>
-      <c r="L393" t="inlineStr"/>
+      <c r="L393" t="inlineStr">
+        <is>
+          <t>A1.01</t>
+        </is>
+      </c>
       <c r="M393" t="inlineStr"/>
       <c r="N393" t="n">
         <v>-32.1193155</v>
@@ -30325,7 +30425,11 @@
           <t>grocery_or_supermarket, food, point_of_interest, store, establishment</t>
         </is>
       </c>
-      <c r="G394" t="inlineStr"/>
+      <c r="G394" t="inlineStr">
+        <is>
+          <t>Food Production and Preparation</t>
+        </is>
+      </c>
       <c r="H394" t="inlineStr"/>
       <c r="I394" t="inlineStr"/>
       <c r="J394" t="inlineStr"/>
@@ -30730,12 +30834,28 @@
           <t>grocery_or_supermarket, supermarket, food, point_of_interest, store, establishment</t>
         </is>
       </c>
-      <c r="G399" t="inlineStr"/>
-      <c r="H399" t="inlineStr"/>
+      <c r="G399" t="inlineStr">
+        <is>
+          <t>FOOD RETAIL</t>
+        </is>
+      </c>
+      <c r="H399" t="inlineStr">
+        <is>
+          <t>Supermarket/grocery store</t>
+        </is>
+      </c>
       <c r="I399" t="inlineStr"/>
-      <c r="J399" t="inlineStr"/>
+      <c r="J399" t="inlineStr">
+        <is>
+          <t>Supermarket</t>
+        </is>
+      </c>
       <c r="K399" t="inlineStr"/>
-      <c r="L399" t="inlineStr"/>
+      <c r="L399" t="inlineStr">
+        <is>
+          <t>A1.01</t>
+        </is>
+      </c>
       <c r="M399" t="inlineStr"/>
       <c r="N399" t="n">
         <v>-32.1542767</v>
@@ -31775,7 +31895,11 @@
           <t>grocery_or_supermarket, point_of_interest, store, food, establishment</t>
         </is>
       </c>
-      <c r="G412" t="inlineStr"/>
+      <c r="G412" t="inlineStr">
+        <is>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
+        </is>
+      </c>
       <c r="H412" t="inlineStr"/>
       <c r="I412" t="inlineStr"/>
       <c r="J412" t="inlineStr"/>
@@ -32002,7 +32126,11 @@
           <t>grocery_or_supermarket, store, food, point_of_interest, establishment</t>
         </is>
       </c>
-      <c r="G415" t="inlineStr"/>
+      <c r="G415" t="inlineStr">
+        <is>
+          <t>FOOD RETAIL</t>
+        </is>
+      </c>
       <c r="H415" t="inlineStr"/>
       <c r="I415" t="inlineStr"/>
       <c r="J415" t="inlineStr"/>
@@ -33146,7 +33274,7 @@
       </c>
       <c r="G429" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H429" t="inlineStr"/>
@@ -33711,12 +33839,28 @@
           <t>grocery_or_supermarket, supermarket, store, point_of_interest, food, establishment</t>
         </is>
       </c>
-      <c r="G436" t="inlineStr"/>
-      <c r="H436" t="inlineStr"/>
+      <c r="G436" t="inlineStr">
+        <is>
+          <t>FOOD RETAIL</t>
+        </is>
+      </c>
+      <c r="H436" t="inlineStr">
+        <is>
+          <t>Supermarket/grocery store</t>
+        </is>
+      </c>
       <c r="I436" t="inlineStr"/>
-      <c r="J436" t="inlineStr"/>
+      <c r="J436" t="inlineStr">
+        <is>
+          <t>Supermarket</t>
+        </is>
+      </c>
       <c r="K436" t="inlineStr"/>
-      <c r="L436" t="inlineStr"/>
+      <c r="L436" t="inlineStr">
+        <is>
+          <t>A1.01</t>
+        </is>
+      </c>
       <c r="M436" t="inlineStr"/>
       <c r="N436" t="n">
         <v>-32.1266869</v>
@@ -33861,7 +34005,11 @@
           <t>food, point_of_interest, establishment</t>
         </is>
       </c>
-      <c r="G438" t="inlineStr"/>
+      <c r="G438" t="inlineStr">
+        <is>
+          <t>Food Production and Preparation</t>
+        </is>
+      </c>
       <c r="H438" t="inlineStr"/>
       <c r="I438" t="inlineStr"/>
       <c r="J438" t="inlineStr"/>
@@ -34254,12 +34402,28 @@
           <t>grocery_or_supermarket, supermarket, store, food, point_of_interest, establishment</t>
         </is>
       </c>
-      <c r="G443" t="inlineStr"/>
-      <c r="H443" t="inlineStr"/>
+      <c r="G443" t="inlineStr">
+        <is>
+          <t>FOOD RETAIL</t>
+        </is>
+      </c>
+      <c r="H443" t="inlineStr">
+        <is>
+          <t>Supermarket/grocery store</t>
+        </is>
+      </c>
       <c r="I443" t="inlineStr"/>
-      <c r="J443" t="inlineStr"/>
+      <c r="J443" t="inlineStr">
+        <is>
+          <t>Supermarket</t>
+        </is>
+      </c>
       <c r="K443" t="inlineStr"/>
-      <c r="L443" t="inlineStr"/>
+      <c r="L443" t="inlineStr">
+        <is>
+          <t>A1.01</t>
+        </is>
+      </c>
       <c r="M443" t="inlineStr"/>
       <c r="N443" t="n">
         <v>-32.1149849</v>
@@ -34558,7 +34722,11 @@
           <t>food, point_of_interest, establishment</t>
         </is>
       </c>
-      <c r="G447" t="inlineStr"/>
+      <c r="G447" t="inlineStr">
+        <is>
+          <t>Food Production and Preparation</t>
+        </is>
+      </c>
       <c r="H447" t="inlineStr"/>
       <c r="I447" t="inlineStr"/>
       <c r="J447" t="inlineStr"/>
@@ -34955,7 +35123,11 @@
           <t>grocery_or_supermarket, point_of_interest, store, food, establishment</t>
         </is>
       </c>
-      <c r="G452" t="inlineStr"/>
+      <c r="G452" t="inlineStr">
+        <is>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
+        </is>
+      </c>
       <c r="H452" t="inlineStr"/>
       <c r="I452" t="inlineStr"/>
       <c r="J452" t="inlineStr"/>
@@ -35194,7 +35366,11 @@
           <t>grocery_or_supermarket, food, point_of_interest, store, establishment</t>
         </is>
       </c>
-      <c r="G455" t="inlineStr"/>
+      <c r="G455" t="inlineStr">
+        <is>
+          <t>Food Production and Preparation</t>
+        </is>
+      </c>
       <c r="H455" t="inlineStr"/>
       <c r="I455" t="inlineStr"/>
       <c r="J455" t="inlineStr"/>
@@ -35344,7 +35520,11 @@
           <t>food, point_of_interest, store, establishment</t>
         </is>
       </c>
-      <c r="G457" t="inlineStr"/>
+      <c r="G457" t="inlineStr">
+        <is>
+          <t>Food Production and Preparation</t>
+        </is>
+      </c>
       <c r="H457" t="inlineStr"/>
       <c r="I457" t="inlineStr"/>
       <c r="J457" t="inlineStr"/>
@@ -35899,12 +36079,28 @@
           <t>grocery_or_supermarket, supermarket, food, store, point_of_interest, establishment</t>
         </is>
       </c>
-      <c r="G464" t="inlineStr"/>
-      <c r="H464" t="inlineStr"/>
+      <c r="G464" t="inlineStr">
+        <is>
+          <t>FOOD RETAIL</t>
+        </is>
+      </c>
+      <c r="H464" t="inlineStr">
+        <is>
+          <t>Supermarket/grocery store</t>
+        </is>
+      </c>
       <c r="I464" t="inlineStr"/>
-      <c r="J464" t="inlineStr"/>
+      <c r="J464" t="inlineStr">
+        <is>
+          <t>Supermarket</t>
+        </is>
+      </c>
       <c r="K464" t="inlineStr"/>
-      <c r="L464" t="inlineStr"/>
+      <c r="L464" t="inlineStr">
+        <is>
+          <t>A1.01</t>
+        </is>
+      </c>
       <c r="M464" t="inlineStr"/>
       <c r="N464" t="n">
         <v>-32.1145691</v>
@@ -36523,12 +36719,28 @@
           <t>grocery_or_supermarket, supermarket, home_goods_store, store, food, point_of_interest, establishment</t>
         </is>
       </c>
-      <c r="G472" t="inlineStr"/>
-      <c r="H472" t="inlineStr"/>
+      <c r="G472" t="inlineStr">
+        <is>
+          <t>FOOD RETAIL</t>
+        </is>
+      </c>
+      <c r="H472" t="inlineStr">
+        <is>
+          <t>Supermarket/grocery store</t>
+        </is>
+      </c>
       <c r="I472" t="inlineStr"/>
-      <c r="J472" t="inlineStr"/>
+      <c r="J472" t="inlineStr">
+        <is>
+          <t>Supermarket</t>
+        </is>
+      </c>
       <c r="K472" t="inlineStr"/>
-      <c r="L472" t="inlineStr"/>
+      <c r="L472" t="inlineStr">
+        <is>
+          <t>A1.01</t>
+        </is>
+      </c>
       <c r="M472" t="inlineStr"/>
       <c r="N472" t="n">
         <v>-32.1308393</v>
@@ -36679,7 +36891,7 @@
       </c>
       <c r="G474" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H474" t="inlineStr"/>
@@ -36750,7 +36962,11 @@
           <t>food, point_of_interest, store, establishment</t>
         </is>
       </c>
-      <c r="G475" t="inlineStr"/>
+      <c r="G475" t="inlineStr">
+        <is>
+          <t>Food Production and Preparation</t>
+        </is>
+      </c>
       <c r="H475" t="inlineStr"/>
       <c r="I475" t="inlineStr"/>
       <c r="J475" t="inlineStr"/>
@@ -37052,7 +37268,7 @@
       </c>
       <c r="G479" t="inlineStr">
         <is>
-          <t>FOOD RETAI,FOOD SERVICE</t>
+          <t>FOOD RETAI,FOOD SERVICE,Food Production and Preparation</t>
         </is>
       </c>
       <c r="H479" t="inlineStr"/>
@@ -37597,7 +37813,11 @@
           <t>food, point_of_interest, store, establishment</t>
         </is>
       </c>
-      <c r="G486" t="inlineStr"/>
+      <c r="G486" t="inlineStr">
+        <is>
+          <t>Food Production and Preparation</t>
+        </is>
+      </c>
       <c r="H486" t="inlineStr"/>
       <c r="I486" t="inlineStr"/>
       <c r="J486" t="inlineStr"/>

</xml_diff>